<commit_message>
results of the R workshop day, project finished
</commit_message>
<xml_diff>
--- a/ACRPrecipVsYield.xlsx
+++ b/ACRPrecipVsYield.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/christopher_brackett_usda_gov/Documents/Documents/Data foundations camp/Data-foundations-camp-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85fa95e812e515ab/Documents/GitHub/Data-foundations-camp-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{CCD0C72A-2BC7-43D3-92EC-6A560B2EDD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4302F221-71F9-43AC-B542-545EFAE8B807}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{CCD0C72A-2BC7-43D3-92EC-6A560B2EDD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B16D8FA-1E3D-44D9-9D0B-EFD8F8812784}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="96" windowWidth="11712" windowHeight="12240" activeTab="1" xr2:uid="{255772B1-BE5E-478E-8A8E-916C17154AD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{255772B1-BE5E-478E-8A8E-916C17154AD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="121">
   <si>
     <t>year</t>
   </si>
@@ -406,7 +407,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,12 +421,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -788,20 +783,20 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -812,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1995</v>
       </c>
@@ -823,7 +818,7 @@
         <v>2045.605136666667</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1996</v>
       </c>
@@ -834,7 +829,7 @@
         <v>4369.8660133333324</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>2000</v>
       </c>
@@ -845,7 +840,7 @@
         <v>596.65506999999991</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -856,7 +851,7 @@
         <v>4530.4536199999993</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>2003</v>
       </c>
@@ -867,7 +862,7 @@
         <v>3075.7496000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -878,7 +873,7 @@
         <v>5675.1167000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -889,7 +884,7 @@
         <v>3116.8492666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -900,7 +895,7 @@
         <v>2215.6456666666668</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>2015</v>
       </c>
@@ -911,7 +906,7 @@
         <v>1219.1655666666668</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -922,7 +917,7 @@
         <v>4896.0911999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2017</v>
       </c>
@@ -933,12 +928,12 @@
         <v>3980.3159000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -949,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>1997</v>
       </c>
@@ -960,7 +955,7 @@
         <v>422.35511999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1998</v>
       </c>
@@ -971,7 +966,7 @@
         <v>3313.4551266666663</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1999</v>
       </c>
@@ -982,7 +977,7 @@
         <v>5279.812633333333</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>2002</v>
       </c>
@@ -993,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -1004,7 +999,7 @@
         <v>3098.5412333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2006</v>
       </c>
@@ -1015,7 +1010,7 @@
         <v>1435.4992666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>2009</v>
       </c>
@@ -1026,7 +1021,7 @@
         <v>2834.7561000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>2012</v>
       </c>
@@ -1037,7 +1032,7 @@
         <v>87.80383333333333</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -1048,7 +1043,7 @@
         <v>3108.2557000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>2007</v>
       </c>
@@ -1059,7 +1054,7 @@
         <v>3485.6253666666667</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -1070,7 +1065,7 @@
         <v>3245.0055000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>2005</v>
       </c>
@@ -1087,16 +1082,296 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BC9798-5884-4549-AEAF-F62E796D62BB}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1995</v>
+      </c>
+      <c r="B2">
+        <v>30.225999999999996</v>
+      </c>
+      <c r="C2">
+        <v>2045.605136666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1996</v>
+      </c>
+      <c r="B3">
+        <v>76.2</v>
+      </c>
+      <c r="C3">
+        <v>4369.8660133333324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>70.103999999999985</v>
+      </c>
+      <c r="C4">
+        <v>596.65506999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>2001</v>
+      </c>
+      <c r="B5">
+        <v>95.630999999999972</v>
+      </c>
+      <c r="C5">
+        <v>4530.4536199999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>2003</v>
+      </c>
+      <c r="B6">
+        <v>34.544000000000004</v>
+      </c>
+      <c r="C6">
+        <v>3075.7496000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>2008</v>
+      </c>
+      <c r="B7">
+        <v>188.97599999999997</v>
+      </c>
+      <c r="C7">
+        <v>5675.1167000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>58.673999999999985</v>
+      </c>
+      <c r="C8">
+        <v>3116.8492666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>2011</v>
+      </c>
+      <c r="B9">
+        <v>3.556</v>
+      </c>
+      <c r="C9">
+        <v>2215.6456666666668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B10">
+        <v>105.15599999999999</v>
+      </c>
+      <c r="C10">
+        <v>1219.1655666666668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11">
+        <v>70.103999999999985</v>
+      </c>
+      <c r="C11">
+        <v>4896.0911999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>2017</v>
+      </c>
+      <c r="B12">
+        <v>81.787999999999982</v>
+      </c>
+      <c r="C12">
+        <v>3980.3159000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B13">
+        <v>89.915999999999997</v>
+      </c>
+      <c r="C13">
+        <v>422.35511999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>1998</v>
+      </c>
+      <c r="B14">
+        <v>124.20599999999999</v>
+      </c>
+      <c r="C14">
+        <v>3313.4551266666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>1999</v>
+      </c>
+      <c r="B15">
+        <v>167.13200000000001</v>
+      </c>
+      <c r="C15">
+        <v>5279.812633333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>2002</v>
+      </c>
+      <c r="B16">
+        <v>15.494000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="B17">
+        <v>98.551999999999992</v>
+      </c>
+      <c r="C17">
+        <v>3098.5412333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2006</v>
+      </c>
+      <c r="B18">
+        <v>55.372</v>
+      </c>
+      <c r="C18">
+        <v>1435.4992666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>2009</v>
+      </c>
+      <c r="B19">
+        <v>63.245999999999988</v>
+      </c>
+      <c r="C19">
+        <v>2834.7561000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>25.907999999999998</v>
+      </c>
+      <c r="C20">
+        <v>87.80383333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>94.234000000000009</v>
+      </c>
+      <c r="C21">
+        <v>3108.2557000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>2007</v>
+      </c>
+      <c r="B22">
+        <v>133.09599999999998</v>
+      </c>
+      <c r="C22">
+        <v>3485.6253666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23">
+        <v>129.03199999999998</v>
+      </c>
+      <c r="C23">
+        <v>3245.0055000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>2005</v>
+      </c>
+      <c r="B24">
+        <v>91.947999999999993</v>
+      </c>
+      <c r="C24">
+        <v>2280.2842333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238DEDC0-20E7-493C-8E48-BF6D1F5D966A}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -1169,7 +1444,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1993</v>
       </c>
@@ -1201,7 +1476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1993</v>
       </c>
@@ -1233,7 +1508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1994</v>
       </c>
@@ -1265,7 +1540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -1297,7 +1572,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -1329,7 +1604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -1370,7 +1645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>1995</v>
       </c>
@@ -1411,7 +1686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1995</v>
       </c>
@@ -1452,7 +1727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>1996</v>
       </c>
@@ -1493,7 +1768,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>1996</v>
       </c>
@@ -1534,7 +1809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>1996</v>
       </c>
@@ -1575,7 +1850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>1997</v>
       </c>
@@ -1616,7 +1891,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>1997</v>
       </c>
@@ -1657,7 +1932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>1997</v>
       </c>
@@ -1698,7 +1973,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>1998</v>
       </c>
@@ -1739,7 +2014,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>1998</v>
       </c>
@@ -1780,7 +2055,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>1998</v>
       </c>
@@ -1821,7 +2096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>1999</v>
       </c>
@@ -1862,7 +2137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>1999</v>
       </c>
@@ -1903,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>1999</v>
       </c>
@@ -1944,7 +2219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>2000</v>
       </c>
@@ -1985,7 +2260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>2000</v>
       </c>
@@ -2026,7 +2301,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -2067,7 +2342,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>2001</v>
       </c>
@@ -2108,7 +2383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>2001</v>
       </c>
@@ -2149,7 +2424,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>2001</v>
       </c>
@@ -2190,7 +2465,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>2002</v>
       </c>
@@ -2231,7 +2506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>2002</v>
       </c>
@@ -2272,7 +2547,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>2002</v>
       </c>
@@ -2313,7 +2588,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>2003</v>
       </c>
@@ -2354,7 +2629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>2003</v>
       </c>
@@ -2395,7 +2670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>2003</v>
       </c>
@@ -2436,7 +2711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>2004</v>
       </c>
@@ -2477,7 +2752,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -2518,7 +2793,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>2004</v>
       </c>
@@ -2559,7 +2834,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>2005</v>
       </c>
@@ -2600,7 +2875,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>2005</v>
       </c>
@@ -2641,7 +2916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40">
         <v>2005</v>
       </c>
@@ -2682,7 +2957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13">
       <c r="A41">
         <v>2006</v>
       </c>
@@ -2723,7 +2998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>2006</v>
       </c>
@@ -2764,7 +3039,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>2006</v>
       </c>
@@ -2805,7 +3080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
       <c r="A44">
         <v>2007</v>
       </c>
@@ -2846,7 +3121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45">
         <v>2007</v>
       </c>
@@ -2887,7 +3162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13">
       <c r="A46">
         <v>2007</v>
       </c>
@@ -2928,7 +3203,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13">
       <c r="A47">
         <v>2008</v>
       </c>
@@ -2969,7 +3244,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13">
       <c r="A48">
         <v>2008</v>
       </c>
@@ -3010,7 +3285,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13">
       <c r="A49">
         <v>2008</v>
       </c>
@@ -3051,7 +3326,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13">
       <c r="A50">
         <v>2009</v>
       </c>
@@ -3092,7 +3367,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13">
       <c r="A51">
         <v>2009</v>
       </c>
@@ -3133,7 +3408,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13">
       <c r="A52">
         <v>2009</v>
       </c>
@@ -3174,7 +3449,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13">
       <c r="A53">
         <v>2010</v>
       </c>
@@ -3215,7 +3490,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13">
       <c r="A54">
         <v>2010</v>
       </c>
@@ -3256,7 +3531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13">
       <c r="A55">
         <v>2010</v>
       </c>
@@ -3297,7 +3572,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -3338,7 +3613,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -3379,7 +3654,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13">
       <c r="A58">
         <v>2011</v>
       </c>
@@ -3420,7 +3695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13">
       <c r="A59">
         <v>2012</v>
       </c>
@@ -3461,7 +3736,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13">
       <c r="A60">
         <v>2012</v>
       </c>
@@ -3502,7 +3777,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13">
       <c r="A61">
         <v>2012</v>
       </c>
@@ -3543,7 +3818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13">
       <c r="A62">
         <v>2013</v>
       </c>
@@ -3584,7 +3859,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13">
       <c r="A63">
         <v>2013</v>
       </c>
@@ -3625,7 +3900,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13">
       <c r="A64">
         <v>2013</v>
       </c>
@@ -3666,7 +3941,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13">
       <c r="A65">
         <v>2014</v>
       </c>
@@ -3707,7 +3982,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13">
       <c r="A66">
         <v>2014</v>
       </c>
@@ -3748,7 +4023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13">
       <c r="A67">
         <v>2014</v>
       </c>
@@ -3789,7 +4064,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13">
       <c r="A68">
         <v>2015</v>
       </c>
@@ -3830,7 +4105,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13">
       <c r="A69">
         <v>2015</v>
       </c>
@@ -3871,7 +4146,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13">
       <c r="A70">
         <v>2015</v>
       </c>
@@ -3912,7 +4187,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13">
       <c r="A71">
         <v>2016</v>
       </c>
@@ -3953,7 +4228,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13">
       <c r="A72">
         <v>2016</v>
       </c>
@@ -3994,7 +4269,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13">
       <c r="A73">
         <v>2016</v>
       </c>
@@ -4035,7 +4310,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13">
       <c r="A74">
         <v>2017</v>
       </c>
@@ -4076,7 +4351,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13">
       <c r="A75">
         <v>2017</v>
       </c>
@@ -4117,7 +4392,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13">
       <c r="A76">
         <v>2017</v>
       </c>

</xml_diff>